<commit_message>
implement microsporidia species + host predictions, organized some papers
</commit_message>
<xml_diff>
--- a/data/manually_collect_abstracts.xlsx
+++ b/data/manually_collect_abstracts.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">year_first_described</t>
   </si>
   <si>
-    <t xml:space="preserve">first_paper_reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">first_paper_title</t>
+    <t xml:space="preserve">paper_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paper_title</t>
   </si>
   <si>
     <t xml:space="preserve">abstract</t>
@@ -2209,7 +2209,7 @@
     <t xml:space="preserve">Новая микроспоридия Alfvenia ceriodaphniae sp. n. из Ceriodaphnia reticulata (Crustacea: Cladocera). :7.Видтманн СС, Соколова ЮЯ, Vidtmann SS, Sokolova YY. Новая микроспоридия Alfvenia ceriodaphniae sp. n. из Ceriodaphnia reticulata (Crustacea: Cladocera)</t>
   </si>
   <si>
-    <t xml:space="preserve">On the basis of electronmicroscopic data the description of Alfvenia ceriodaphniae sp. n. from Ceriodaphnia reticulata (Crustacea, Cladocera) is presented. The nuclear apparatus of meronts is diplokariotic. Sporonts, sporoblasts and spores are uninuclear. The sporogonial Plasmodium undertakes the rosette-like division with the formation of sporoblasts. Spores are egg-shaped, their size: 4.5(4.2-4.8) X X 3.3(2.9-3.5) ц т . Evry spore lays individually inside the envelope, that is formed from the external layer of the sporoblast wall. Polar tube is isofillar, forming 8 - 9 coils. Polaroplast is consisted of the lamellar and chamber parts. The site of parasite localisation is crustacean hypoderm.</t>
+    <t xml:space="preserve">On the basis of electronmicroscopic data the description of Alfvenia ceriodaphniae sp. n. from Ceriodaphnia reticulata (Crustacea, Cladocera) is presented. The nuclear apparatus of meronts is diplokariotic. Sporonts, sporoblasts and spores are uninuclear. The sporogonial Plasmodium undertakes the rosette-like division with the formation of sporoblasts. Spores are egg-shaped, their size: 4.5(4.2-4.8) X 3.3(2.9-3.5) ц т . Evry spore lays individually inside the envelope, that is formed from the external layer of the sporoblast wall. Polar tube is isofillar, forming 8 - 9 coils. Polaroplast is consisted of the lamellar and chamber parts. The site of parasite localisation is crustacean hypoderm.</t>
   </si>
   <si>
     <t xml:space="preserve">Amblyospora egypti</t>
@@ -6994,7 +6994,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -7042,11 +7042,6 @@
       <name val="Liberation Sans;Arial"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -7148,7 +7143,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7201,23 +7196,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7309,12 +7300,12 @@
   <dimension ref="A1:G635"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="D558" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="D2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A558" activeCellId="0" sqref="A558"/>
+      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.28"/>
@@ -8134,7 +8125,7 @@
       <c r="C45" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="9" t="s">
         <v>167</v>
       </c>
       <c r="E45" s="0" t="s">
@@ -8171,7 +8162,7 @@
       <c r="D47" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="12" t="s">
         <v>177</v>
       </c>
     </row>
@@ -8188,7 +8179,7 @@
       <c r="D48" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="12" t="s">
         <v>177</v>
       </c>
     </row>
@@ -8486,7 +8477,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="13" t="s">
         <v>221</v>
       </c>
       <c r="B66" s="0" t="n">
@@ -8498,7 +8489,7 @@
       <c r="D66" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="14" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8605,7 +8596,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="13" t="s">
         <v>247</v>
       </c>
       <c r="B73" s="0" t="n">
@@ -10257,7 +10248,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="14" t="s">
+      <c r="A166" s="13" t="s">
         <v>551</v>
       </c>
       <c r="B166" s="0" t="n">
@@ -10275,7 +10266,7 @@
       <c r="G166" s="7"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="16" t="s">
+      <c r="A167" s="15" t="s">
         <v>555</v>
       </c>
       <c r="B167" s="0" t="n">
@@ -10523,7 +10514,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="14" t="s">
+      <c r="A181" s="13" t="s">
         <v>598</v>
       </c>
       <c r="B181" s="0" t="n">
@@ -10711,7 +10702,7 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="14" t="s">
+      <c r="A192" s="13" t="s">
         <v>633</v>
       </c>
       <c r="B192" s="0" t="n">
@@ -10979,7 +10970,7 @@
       <c r="B207" s="0" t="n">
         <v>1991</v>
       </c>
-      <c r="C207" s="17" t="s">
+      <c r="C207" s="16" t="s">
         <v>684</v>
       </c>
       <c r="D207" s="0" t="s">
@@ -15367,7 +15358,7 @@
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="14" t="s">
+      <c r="A455" s="13" t="s">
         <v>1531</v>
       </c>
       <c r="B455" s="0" t="n">
@@ -15381,7 +15372,7 @@
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A456" s="14" t="s">
+      <c r="A456" s="13" t="s">
         <v>1534</v>
       </c>
       <c r="B456" s="0" t="n">
@@ -15395,7 +15386,7 @@
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A457" s="14" t="s">
+      <c r="A457" s="13" t="s">
         <v>1535</v>
       </c>
       <c r="B457" s="0" t="n">
@@ -17106,7 +17097,7 @@
       <c r="B558" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="C558" s="18" t="s">
+      <c r="C558" s="17" t="s">
         <v>1871</v>
       </c>
       <c r="D558" s="0" t="s">
@@ -18373,7 +18364,7 @@
       <c r="C632" s="0" t="s">
         <v>2121</v>
       </c>
-      <c r="D632" s="19" t="s">
+      <c r="D632" s="18" t="s">
         <v>2122</v>
       </c>
       <c r="E632" s="0" t="s">

</xml_diff>